<commit_message>
Radiation Met Ids set
</commit_message>
<xml_diff>
--- a/Documentation/MetIDs.xlsx
+++ b/Documentation/MetIDs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E342E074-7201-424F-AFE4-0D6A5F889F31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4CA36C-8F7E-4EE0-911D-B84D835B0CDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8263" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="127">
   <si>
     <t>NetID</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>Player (7)</t>
+  </si>
+  <si>
+    <t>Radiation</t>
+  </si>
+  <si>
+    <t>Games</t>
   </si>
 </sst>
 </file>
@@ -774,9 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B442" sqref="B442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3705,11 +3711,21 @@
       <c r="A241">
         <v>240</v>
       </c>
-      <c r="B241" s="11"/>
-      <c r="C241" s="11"/>
-      <c r="D241" s="11"/>
-      <c r="E241" s="11"/>
-      <c r="F241" s="10"/>
+      <c r="B241" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C241" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D241" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E241" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F241" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A242">
@@ -5424,13 +5440,21 @@
       <c r="A441">
         <v>440</v>
       </c>
-      <c r="B441" t="s">
-        <v>21</v>
-      </c>
-      <c r="C441" s="11"/>
-      <c r="D441" s="11"/>
-      <c r="E441" s="11"/>
-      <c r="F441" s="10"/>
+      <c r="B441" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C441" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D441" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E441" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F441" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A442">

</xml_diff>